<commit_message>
amen version of the app added
</commit_message>
<xml_diff>
--- a/budget-viz-tool/working-data/cost_data_HS_inc1b.xlsx
+++ b/budget-viz-tool/working-data/cost_data_HS_inc1b.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hslater\Box\nigeria-data-analytics\budget-viz-tool\nigeria-budget-viz-tool-main\nigeria-budget-viz-tool-main\prep for AMEN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hthompson\Documents\github\nigeria-budget-viz-tool\budget-viz-tool\working-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DB3364E-622D-41FA-9EE1-7B0059862BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0109105E-3CDB-41A1-B41F-9A6FEA75B509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6D501097-96B5-4E3D-B136-E02BA2215B67}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6D501097-96B5-4E3D-B136-E02BA2215B67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,20 +578,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1F1EC2-9D24-491F-AB27-BD88A2530A55}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="48" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -625,7 +625,7 @@
         <v>216887893</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -642,7 +642,7 @@
         <v>159001003</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -659,7 +659,7 @@
         <v>14634797</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -676,7 +676,7 @@
         <v>266113441</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -693,7 +693,7 @@
         <v>73609062</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
@@ -704,13 +704,13 @@
         <v>37</v>
       </c>
       <c r="D7" s="10">
-        <v>37</v>
+        <v>774</v>
       </c>
       <c r="E7" s="11">
         <v>158838186</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -727,7 +727,7 @@
         <v>133056720</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -744,7 +744,7 @@
         <v>31783748</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -761,7 +761,7 @@
         <v>60447808</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
@@ -778,7 +778,7 @@
         <v>127067311</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -791,7 +791,7 @@
         <v>10962296</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -804,7 +804,7 @@
         <v>4702569</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -817,7 +817,7 @@
         <v>5698839</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
@@ -830,7 +830,7 @@
         <v>65906</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -843,7 +843,7 @@
         <v>9329850</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>19</v>
       </c>
@@ -858,7 +858,7 @@
         <v>2200000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
@@ -875,7 +875,7 @@
         <v>43377579</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>5</v>
       </c>
@@ -892,7 +892,7 @@
         <v>159001003</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>6</v>
       </c>
@@ -909,7 +909,7 @@
         <v>14634797</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>7</v>
       </c>
@@ -926,7 +926,7 @@
         <v>250913403</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -943,7 +943,7 @@
         <v>45106220</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>9</v>
       </c>
@@ -960,7 +960,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -977,7 +977,7 @@
         <v>51658642</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
@@ -994,7 +994,7 @@
         <v>5412309</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>60447808</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>73078040</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>14</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>10962296</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>4702569</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>16</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>5698839</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>17</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>65906</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>18</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>9329850</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>19</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>930769</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>4</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>21688789</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>159001003</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>14634797</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>250913403</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>8</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>45106220</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>9</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>10</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>51658642</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>11</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>5412309</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>12</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>60447808</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>4360283</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>10962296</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" ht="32" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>15</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>4702569</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>16</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>5698839</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>17</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>65906</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>18</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>9329850</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>19</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>930769</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
         <v>4</v>
       </c>
@@ -1369,7 +1369,7 @@
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>5</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>159001003</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>14634797</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>7</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>250913403</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>8</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>50337812</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>9</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" ht="22.5" x14ac:dyDescent="0.45">
       <c r="A56" s="5" t="s">
         <v>10</v>
       </c>
@@ -1465,7 +1465,7 @@
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
     </row>
-    <row r="57" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>11</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>5412309</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>12</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>60447808</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>13</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>4360283</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>14</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>10962296</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>15</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>4702569</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>16</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>5698839</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>17</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>65906</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>18</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>9329850</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>